<commit_message>
moving things to data package2
</commit_message>
<xml_diff>
--- a/data/raw/eugene-raw.xlsx
+++ b/data/raw/eugene-raw.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\au757887\PC_documents\_git-it\ghproj_CENTS\data\raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D874138A-BD10-4360-9DF1-C26AAFF6629C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7573F42-F07D-40CC-9B4F-D4CCD268E147}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{CBE61150-97A6-4917-A64E-10F8CCC916BE}"/>
+    <workbookView xWindow="24" yWindow="624" windowWidth="23016" windowHeight="12336" xr2:uid="{CBE61150-97A6-4917-A64E-10F8CCC916BE}"/>
   </bookViews>
   <sheets>
     <sheet name="Ark1" sheetId="1" r:id="rId1"/>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="371" uniqueCount="63">
   <si>
     <t>Location</t>
   </si>
@@ -224,6 +224,15 @@
   </si>
   <si>
     <t>H</t>
+  </si>
+  <si>
+    <t>The correct dates are,</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Plowing  R3 R4                         28-11-2019 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Harrowing 8-10 cm  R3 R4      04-04-2019 </t>
   </si>
 </sst>
 </file>
@@ -233,7 +242,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="dd\-mmm\-yy"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -245,11 +254,13 @@
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
@@ -267,6 +278,12 @@
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -393,13 +410,10 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyAlignment="1">
@@ -425,6 +439,9 @@
     </xf>
     <xf numFmtId="2" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -473,23 +490,23 @@
       <sheetName val="Ark1"/>
     </sheetNames>
     <sheetDataSet>
-      <sheetData sheetId="0" refreshError="1"/>
-      <sheetData sheetId="1" refreshError="1"/>
-      <sheetData sheetId="2" refreshError="1"/>
-      <sheetData sheetId="3" refreshError="1"/>
-      <sheetData sheetId="4" refreshError="1"/>
-      <sheetData sheetId="5" refreshError="1"/>
-      <sheetData sheetId="6" refreshError="1"/>
-      <sheetData sheetId="7" refreshError="1"/>
-      <sheetData sheetId="8" refreshError="1"/>
-      <sheetData sheetId="9" refreshError="1"/>
-      <sheetData sheetId="10" refreshError="1"/>
-      <sheetData sheetId="11" refreshError="1"/>
-      <sheetData sheetId="12" refreshError="1"/>
-      <sheetData sheetId="13" refreshError="1"/>
-      <sheetData sheetId="14" refreshError="1"/>
-      <sheetData sheetId="15" refreshError="1"/>
-      <sheetData sheetId="16" refreshError="1"/>
+      <sheetData sheetId="0"/>
+      <sheetData sheetId="1"/>
+      <sheetData sheetId="2"/>
+      <sheetData sheetId="3"/>
+      <sheetData sheetId="4"/>
+      <sheetData sheetId="5"/>
+      <sheetData sheetId="6"/>
+      <sheetData sheetId="7"/>
+      <sheetData sheetId="8"/>
+      <sheetData sheetId="9"/>
+      <sheetData sheetId="10"/>
+      <sheetData sheetId="11"/>
+      <sheetData sheetId="12"/>
+      <sheetData sheetId="13"/>
+      <sheetData sheetId="14"/>
+      <sheetData sheetId="15"/>
+      <sheetData sheetId="16"/>
       <sheetData sheetId="17">
         <row r="2">
           <cell r="R2" t="str">
@@ -557,6 +574,7 @@
           <cell r="N12" t="str">
             <v>Gødning 15 kg N/ha efterår + (1,00 norm – 15 kg N/ha) forår</v>
           </cell>
+          <cell r="R12"/>
         </row>
         <row r="13">
           <cell r="N13" t="str">
@@ -624,7 +642,7 @@
           </cell>
         </row>
       </sheetData>
-      <sheetData sheetId="18" refreshError="1"/>
+      <sheetData sheetId="18"/>
     </sheetDataSet>
   </externalBook>
 </externalLink>
@@ -949,8 +967,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{40E1473E-FA14-4D23-9DD4-60D70CE4DF5B}">
   <dimension ref="A1:O349"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D55" sqref="D55:F56"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G87" sqref="G87:G90"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2250,36 +2268,36 @@
       <c r="F57" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="G57" s="9" t="s">
+      <c r="G57" s="7" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="58" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A58" s="9"/>
-      <c r="B58" s="9"/>
-      <c r="C58" s="9"/>
-      <c r="D58" s="9"/>
+      <c r="A58" s="7"/>
+      <c r="B58" s="7"/>
+      <c r="C58" s="7"/>
+      <c r="D58" s="7"/>
       <c r="E58" s="8"/>
-      <c r="F58" s="9"/>
-      <c r="G58" s="9"/>
+      <c r="F58" s="7"/>
+      <c r="G58" s="7"/>
     </row>
     <row r="59" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A59" s="9"/>
-      <c r="B59" s="9"/>
-      <c r="C59" s="9"/>
-      <c r="D59" s="9"/>
+      <c r="A59" s="7"/>
+      <c r="B59" s="7"/>
+      <c r="C59" s="7"/>
+      <c r="D59" s="7"/>
       <c r="E59" s="8"/>
-      <c r="F59" s="9"/>
-      <c r="G59" s="9"/>
+      <c r="F59" s="7"/>
+      <c r="G59" s="7"/>
     </row>
     <row r="60" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A60" s="9"/>
-      <c r="B60" s="9"/>
-      <c r="C60" s="9"/>
-      <c r="D60" s="9"/>
+      <c r="A60" s="7"/>
+      <c r="B60" s="7"/>
+      <c r="C60" s="7"/>
+      <c r="D60" s="7"/>
       <c r="E60" s="8"/>
-      <c r="F60" s="9"/>
-      <c r="G60" s="9"/>
+      <c r="F60" s="7"/>
+      <c r="G60" s="7"/>
     </row>
     <row r="61" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A61" s="2" t="s">
@@ -2369,7 +2387,7 @@
       <c r="M63" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="N63" s="10"/>
+      <c r="N63" s="9"/>
       <c r="O63" s="4" t="s">
         <v>7</v>
       </c>
@@ -2412,7 +2430,7 @@
       <c r="M64" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="N64" s="10"/>
+      <c r="N64" s="9"/>
       <c r="O64" s="4" t="s">
         <v>7</v>
       </c>
@@ -2455,7 +2473,7 @@
       <c r="M65" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="N65" s="10"/>
+      <c r="N65" s="9"/>
       <c r="O65" s="4" t="s">
         <v>7</v>
       </c>
@@ -2498,7 +2516,7 @@
       <c r="M66" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="N66" s="10"/>
+      <c r="N66" s="9"/>
       <c r="O66" s="4" t="s">
         <v>7</v>
       </c>
@@ -2541,50 +2559,50 @@
       <c r="M67" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="N67" s="10"/>
+      <c r="N67" s="9"/>
       <c r="O67" s="4" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="68" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A68" s="11">
-        <v>3</v>
-      </c>
-      <c r="B68" s="11">
-        <v>4</v>
-      </c>
-      <c r="C68" s="11">
+      <c r="A68" s="10">
+        <v>3</v>
+      </c>
+      <c r="B68" s="10">
+        <v>4</v>
+      </c>
+      <c r="C68" s="10">
         <v>1</v>
       </c>
-      <c r="D68" s="11"/>
-      <c r="E68" s="12">
+      <c r="D68" s="10"/>
+      <c r="E68" s="11">
         <v>43560</v>
       </c>
-      <c r="F68" s="11" t="s">
+      <c r="F68" s="10" t="s">
         <v>39</v>
       </c>
       <c r="G68" s="4" t="s">
         <v>42</v>
       </c>
-      <c r="H68" s="11">
+      <c r="H68" s="10">
         <v>152</v>
       </c>
-      <c r="I68" s="11">
+      <c r="I68" s="10">
         <v>41</v>
       </c>
-      <c r="J68" s="11">
+      <c r="J68" s="10">
         <v>95</v>
       </c>
-      <c r="K68" s="11">
+      <c r="K68" s="10">
         <v>12.5</v>
       </c>
-      <c r="L68" s="11">
+      <c r="L68" s="10">
         <v>2.5</v>
       </c>
-      <c r="M68" s="11" t="s">
+      <c r="M68" s="10" t="s">
         <v>7</v>
       </c>
-      <c r="N68" s="10"/>
+      <c r="N68" s="9"/>
       <c r="O68" s="4" t="s">
         <v>7</v>
       </c>
@@ -2605,7 +2623,7 @@
       <c r="F69" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G69" s="13" t="s">
+      <c r="G69" s="12" t="s">
         <v>41</v>
       </c>
       <c r="H69" s="2">
@@ -2640,7 +2658,7 @@
       <c r="F70" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G70" s="13" t="s">
+      <c r="G70" s="12" t="s">
         <v>41</v>
       </c>
       <c r="H70" s="2">
@@ -2655,7 +2673,7 @@
       <c r="K70" s="2">
         <v>12.5</v>
       </c>
-      <c r="L70" s="11">
+      <c r="L70" s="10">
         <v>2.5</v>
       </c>
     </row>
@@ -2675,7 +2693,7 @@
       <c r="F71" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G71" s="13" t="s">
+      <c r="G71" s="12" t="s">
         <v>41</v>
       </c>
       <c r="H71" s="2">
@@ -2710,7 +2728,7 @@
       <c r="F72" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G72" s="13" t="s">
+      <c r="G72" s="12" t="s">
         <v>41</v>
       </c>
       <c r="H72" s="2">
@@ -2725,7 +2743,7 @@
       <c r="K72" s="2">
         <v>25</v>
       </c>
-      <c r="L72" s="11">
+      <c r="L72" s="10">
         <v>2.5</v>
       </c>
     </row>
@@ -2745,7 +2763,7 @@
       <c r="F73" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G73" s="13" t="s">
+      <c r="G73" s="12" t="s">
         <v>41</v>
       </c>
       <c r="H73" s="2">
@@ -2780,7 +2798,7 @@
       <c r="F74" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="G74" s="13" t="s">
+      <c r="G74" s="12" t="s">
         <v>41</v>
       </c>
       <c r="H74" s="2">
@@ -2795,284 +2813,284 @@
       <c r="K74" s="2">
         <v>25</v>
       </c>
-      <c r="L74" s="11">
+      <c r="L74" s="10">
         <v>2.5</v>
       </c>
     </row>
     <row r="75" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A75" s="14">
-        <v>3</v>
-      </c>
-      <c r="B75" s="14">
-        <v>3</v>
-      </c>
-      <c r="C75" s="14">
+      <c r="A75" s="13">
+        <v>3</v>
+      </c>
+      <c r="B75" s="13">
+        <v>3</v>
+      </c>
+      <c r="C75" s="13">
         <v>1</v>
       </c>
-      <c r="D75" s="14"/>
-      <c r="E75" s="15">
+      <c r="D75" s="13"/>
+      <c r="E75" s="14">
         <v>43936</v>
       </c>
-      <c r="F75" s="14" t="s">
+      <c r="F75" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="G75" s="14" t="s">
+      <c r="G75" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="H75" s="14">
+      <c r="H75" s="13">
         <v>280</v>
       </c>
-      <c r="I75" s="14">
+      <c r="I75" s="13">
         <v>488</v>
       </c>
-      <c r="J75" s="14">
+      <c r="J75" s="13">
         <v>90</v>
       </c>
-      <c r="K75" s="14">
+      <c r="K75" s="13">
         <v>12.5</v>
       </c>
-      <c r="L75" s="14">
-        <v>4</v>
-      </c>
-      <c r="M75" s="14" t="s">
+      <c r="L75" s="13">
+        <v>4</v>
+      </c>
+      <c r="M75" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="N75" s="16"/>
-      <c r="O75" s="14" t="s">
+      <c r="N75" s="15"/>
+      <c r="O75" s="13" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="76" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A76" s="14">
-        <v>3</v>
-      </c>
-      <c r="B76" s="14">
-        <v>4</v>
-      </c>
-      <c r="C76" s="14">
+      <c r="A76" s="13">
+        <v>3</v>
+      </c>
+      <c r="B76" s="13">
+        <v>4</v>
+      </c>
+      <c r="C76" s="13">
         <v>1</v>
       </c>
-      <c r="D76" s="14"/>
-      <c r="E76" s="15">
+      <c r="D76" s="13"/>
+      <c r="E76" s="14">
         <v>43936</v>
       </c>
-      <c r="F76" s="14" t="s">
+      <c r="F76" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="G76" s="14" t="s">
+      <c r="G76" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="H76" s="14">
+      <c r="H76" s="13">
         <v>280</v>
       </c>
-      <c r="I76" s="14">
+      <c r="I76" s="13">
         <v>488</v>
       </c>
-      <c r="J76" s="14">
+      <c r="J76" s="13">
         <v>90</v>
       </c>
-      <c r="K76" s="14">
+      <c r="K76" s="13">
         <v>12.5</v>
       </c>
-      <c r="L76" s="14">
-        <v>4</v>
-      </c>
-      <c r="M76" s="14" t="s">
+      <c r="L76" s="13">
+        <v>4</v>
+      </c>
+      <c r="M76" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="N76" s="16"/>
-      <c r="O76" s="14" t="s">
+      <c r="N76" s="15"/>
+      <c r="O76" s="13" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="77" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A77" s="14">
-        <v>3</v>
-      </c>
-      <c r="B77" s="14">
-        <v>3</v>
-      </c>
-      <c r="C77" s="14">
+      <c r="A77" s="13">
+        <v>3</v>
+      </c>
+      <c r="B77" s="13">
+        <v>3</v>
+      </c>
+      <c r="C77" s="13">
         <v>2</v>
       </c>
-      <c r="D77" s="14"/>
-      <c r="E77" s="15">
+      <c r="D77" s="13"/>
+      <c r="E77" s="14">
         <v>43936</v>
       </c>
-      <c r="F77" s="14" t="s">
+      <c r="F77" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="G77" s="14" t="s">
+      <c r="G77" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="H77" s="14">
+      <c r="H77" s="13">
         <v>280</v>
       </c>
-      <c r="I77" s="14">
+      <c r="I77" s="13">
         <v>488</v>
       </c>
-      <c r="J77" s="14">
+      <c r="J77" s="13">
         <v>90</v>
       </c>
-      <c r="K77" s="14">
+      <c r="K77" s="13">
         <v>25</v>
       </c>
-      <c r="L77" s="14">
+      <c r="L77" s="13">
         <v>5</v>
       </c>
-      <c r="M77" s="14" t="s">
+      <c r="M77" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="N77" s="16"/>
-      <c r="O77" s="14" t="s">
+      <c r="N77" s="15"/>
+      <c r="O77" s="13" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="78" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A78" s="14">
-        <v>3</v>
-      </c>
-      <c r="B78" s="14">
-        <v>4</v>
-      </c>
-      <c r="C78" s="14">
+      <c r="A78" s="13">
+        <v>3</v>
+      </c>
+      <c r="B78" s="13">
+        <v>4</v>
+      </c>
+      <c r="C78" s="13">
         <v>2</v>
       </c>
-      <c r="D78" s="14"/>
-      <c r="E78" s="15">
+      <c r="D78" s="13"/>
+      <c r="E78" s="14">
         <v>43936</v>
       </c>
-      <c r="F78" s="14" t="s">
+      <c r="F78" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="G78" s="14" t="s">
+      <c r="G78" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="H78" s="14">
+      <c r="H78" s="13">
         <v>280</v>
       </c>
-      <c r="I78" s="14">
+      <c r="I78" s="13">
         <v>488</v>
       </c>
-      <c r="J78" s="14">
+      <c r="J78" s="13">
         <v>90</v>
       </c>
-      <c r="K78" s="14">
+      <c r="K78" s="13">
         <v>25</v>
       </c>
-      <c r="L78" s="14">
+      <c r="L78" s="13">
         <v>5</v>
       </c>
-      <c r="M78" s="14" t="s">
+      <c r="M78" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="N78" s="16"/>
-      <c r="O78" s="14" t="s">
+      <c r="N78" s="15"/>
+      <c r="O78" s="13" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="79" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A79" s="14">
-        <v>3</v>
-      </c>
-      <c r="B79" s="14">
-        <v>3</v>
-      </c>
-      <c r="C79" s="14">
-        <v>4</v>
-      </c>
-      <c r="D79" s="14"/>
-      <c r="E79" s="15">
+      <c r="A79" s="13">
+        <v>3</v>
+      </c>
+      <c r="B79" s="13">
+        <v>3</v>
+      </c>
+      <c r="C79" s="13">
+        <v>4</v>
+      </c>
+      <c r="D79" s="13"/>
+      <c r="E79" s="14">
         <v>43936</v>
       </c>
-      <c r="F79" s="14" t="s">
+      <c r="F79" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="G79" s="14" t="s">
+      <c r="G79" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="H79" s="14">
+      <c r="H79" s="13">
         <v>280</v>
       </c>
-      <c r="I79" s="14">
+      <c r="I79" s="13">
         <v>488</v>
       </c>
-      <c r="J79" s="14">
+      <c r="J79" s="13">
         <v>90</v>
       </c>
-      <c r="K79" s="14">
+      <c r="K79" s="13">
         <v>25</v>
       </c>
-      <c r="L79" s="14">
+      <c r="L79" s="13">
         <v>5</v>
       </c>
-      <c r="M79" s="14" t="s">
+      <c r="M79" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="N79" s="16"/>
-      <c r="O79" s="14" t="s">
+      <c r="N79" s="15"/>
+      <c r="O79" s="13" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="80" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A80" s="14">
-        <v>3</v>
-      </c>
-      <c r="B80" s="14">
-        <v>4</v>
-      </c>
-      <c r="C80" s="14">
-        <v>4</v>
-      </c>
-      <c r="D80" s="14"/>
-      <c r="E80" s="15">
+      <c r="A80" s="13">
+        <v>3</v>
+      </c>
+      <c r="B80" s="13">
+        <v>4</v>
+      </c>
+      <c r="C80" s="13">
+        <v>4</v>
+      </c>
+      <c r="D80" s="13"/>
+      <c r="E80" s="14">
         <v>43936</v>
       </c>
-      <c r="F80" s="14" t="s">
+      <c r="F80" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="G80" s="14" t="s">
+      <c r="G80" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="H80" s="14">
+      <c r="H80" s="13">
         <v>280</v>
       </c>
-      <c r="I80" s="14">
+      <c r="I80" s="13">
         <v>488</v>
       </c>
-      <c r="J80" s="14">
+      <c r="J80" s="13">
         <v>90</v>
       </c>
-      <c r="K80" s="14">
+      <c r="K80" s="13">
         <v>25</v>
       </c>
-      <c r="L80" s="14">
+      <c r="L80" s="13">
         <v>5</v>
       </c>
-      <c r="M80" s="14" t="s">
+      <c r="M80" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="N80" s="16"/>
-      <c r="O80" s="14" t="s">
+      <c r="N80" s="15"/>
+      <c r="O80" s="13" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="81" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A81" s="9"/>
-      <c r="B81" s="9"/>
-      <c r="C81" s="9"/>
-      <c r="D81" s="9"/>
+      <c r="A81" s="7"/>
+      <c r="B81" s="7"/>
+      <c r="C81" s="7"/>
+      <c r="D81" s="7"/>
       <c r="E81" s="8"/>
-      <c r="F81" s="9"/>
-      <c r="G81" s="9"/>
-      <c r="H81" s="9"/>
-      <c r="I81" s="9"/>
-      <c r="J81" s="9"/>
-      <c r="K81" s="9"/>
-      <c r="L81" s="9"/>
-      <c r="M81" s="9"/>
-      <c r="N81" s="10"/>
-      <c r="O81" s="9"/>
+      <c r="F81" s="7"/>
+      <c r="G81" s="7"/>
+      <c r="H81" s="7"/>
+      <c r="I81" s="7"/>
+      <c r="J81" s="7"/>
+      <c r="K81" s="7"/>
+      <c r="L81" s="7"/>
+      <c r="M81" s="7"/>
+      <c r="N81" s="9"/>
+      <c r="O81" s="7"/>
     </row>
     <row r="83" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A83" s="2" t="s">
@@ -3083,7 +3101,7 @@
       </c>
     </row>
     <row r="84" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A84" s="17">
+      <c r="A84" s="16">
         <v>39.025000000000006</v>
       </c>
       <c r="B84" s="2">
@@ -3094,7 +3112,7 @@
       </c>
     </row>
     <row r="85" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A85" s="17">
+      <c r="A85" s="16">
         <v>41.675000000000004</v>
       </c>
       <c r="B85" s="2">
@@ -3105,7 +3123,7 @@
       </c>
     </row>
     <row r="86" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A86" s="17">
+      <c r="A86" s="16">
         <v>39.137500000000003</v>
       </c>
       <c r="B86" s="2">
@@ -3116,7 +3134,7 @@
       </c>
     </row>
     <row r="87" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A87" s="17">
+      <c r="A87" s="16">
         <v>39.950000000000003</v>
       </c>
       <c r="B87" s="2">
@@ -3125,9 +3143,12 @@
       <c r="C87" s="2" t="s">
         <v>49</v>
       </c>
+      <c r="G87" s="17" t="s">
+        <v>60</v>
+      </c>
     </row>
     <row r="88" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A88" s="17">
+      <c r="A88" s="16">
         <v>40.925000000000004</v>
       </c>
       <c r="B88" s="2">
@@ -3136,9 +3157,10 @@
       <c r="C88" s="2" t="s">
         <v>50</v>
       </c>
+      <c r="G88" s="17"/>
     </row>
     <row r="89" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A89" s="17">
+      <c r="A89" s="16">
         <v>40.099999999999994</v>
       </c>
       <c r="B89" s="2">
@@ -3147,9 +3169,12 @@
       <c r="C89" s="2" t="s">
         <v>48</v>
       </c>
+      <c r="G89" s="17" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="90" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A90" s="17">
+      <c r="A90" s="16">
         <v>42.0625</v>
       </c>
       <c r="B90" s="2">
@@ -3158,9 +3183,12 @@
       <c r="C90" s="2" t="s">
         <v>46</v>
       </c>
+      <c r="G90" s="17" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="91" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A91" s="17">
+      <c r="A91" s="16">
         <v>41.3</v>
       </c>
       <c r="B91" s="2">
@@ -3171,7 +3199,7 @@
       </c>
     </row>
     <row r="92" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A92" s="17">
+      <c r="A92" s="16">
         <v>40.075000000000003</v>
       </c>
       <c r="B92" s="2">
@@ -3182,7 +3210,7 @@
       </c>
     </row>
     <row r="93" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A93" s="17">
+      <c r="A93" s="16">
         <v>41.587499999999991</v>
       </c>
       <c r="B93" s="2">
@@ -3193,7 +3221,7 @@
       </c>
     </row>
     <row r="94" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A94" s="17">
+      <c r="A94" s="16">
         <v>40.799999999999997</v>
       </c>
       <c r="B94" s="2">
@@ -3204,7 +3232,7 @@
       </c>
     </row>
     <row r="95" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A95" s="17">
+      <c r="A95" s="16">
         <v>42.075000000000003</v>
       </c>
       <c r="B95" s="2">
@@ -3215,7 +3243,7 @@
       </c>
     </row>
     <row r="96" spans="1:15" x14ac:dyDescent="0.3">
-      <c r="A96" s="17">
+      <c r="A96" s="16">
         <v>41.287500000000001</v>
       </c>
       <c r="B96" s="2">
@@ -3226,7 +3254,7 @@
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A97" s="17">
+      <c r="A97" s="16">
         <v>44.587500000000006</v>
       </c>
       <c r="B97" s="2">
@@ -3237,7 +3265,7 @@
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A98" s="17">
+      <c r="A98" s="16">
         <v>42.712500000000006</v>
       </c>
       <c r="B98" s="2">
@@ -3248,7 +3276,7 @@
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A99" s="17">
+      <c r="A99" s="16">
         <v>42.612500000000004</v>
       </c>
       <c r="B99" s="2">
@@ -3259,7 +3287,7 @@
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A100" s="17">
+      <c r="A100" s="16">
         <v>43.650000000000006</v>
       </c>
       <c r="B100" s="2">
@@ -3270,7 +3298,7 @@
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A101" s="17">
+      <c r="A101" s="16">
         <v>42.9</v>
       </c>
       <c r="B101" s="2">
@@ -3281,7 +3309,7 @@
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A102" s="17">
+      <c r="A102" s="16">
         <v>42.824999999999996</v>
       </c>
       <c r="B102" s="2">
@@ -3292,7 +3320,7 @@
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A103" s="17">
+      <c r="A103" s="16">
         <v>41.424999999999997</v>
       </c>
       <c r="B103" s="2">
@@ -3303,7 +3331,7 @@
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A104" s="17">
+      <c r="A104" s="16">
         <v>42.699999999999996</v>
       </c>
       <c r="B104" s="2">
@@ -3314,7 +3342,7 @@
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A105" s="17">
+      <c r="A105" s="16">
         <v>41.637500000000003</v>
       </c>
       <c r="B105" s="2">
@@ -3325,7 +3353,7 @@
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A106" s="17">
+      <c r="A106" s="16">
         <v>42.474999999999994</v>
       </c>
       <c r="B106" s="2">
@@ -3336,7 +3364,7 @@
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A107" s="17">
+      <c r="A107" s="16">
         <v>42.674999999999997</v>
       </c>
       <c r="B107" s="2">
@@ -3347,7 +3375,7 @@
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A108" s="17">
+      <c r="A108" s="16">
         <v>41.2</v>
       </c>
       <c r="B108" s="2">
@@ -3358,7 +3386,7 @@
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A109" s="17">
+      <c r="A109" s="16">
         <v>40.649999999999991</v>
       </c>
       <c r="B109" s="2">
@@ -3369,7 +3397,7 @@
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A110" s="17">
+      <c r="A110" s="16">
         <v>40.687500000000007</v>
       </c>
       <c r="B110" s="2">
@@ -3380,7 +3408,7 @@
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A111" s="17">
+      <c r="A111" s="16">
         <v>41.962499999999999</v>
       </c>
       <c r="B111" s="2">
@@ -3391,7 +3419,7 @@
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A112" s="17">
+      <c r="A112" s="16">
         <v>43.212499999999999</v>
       </c>
       <c r="B112" s="2">
@@ -3402,7 +3430,7 @@
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A113" s="17">
+      <c r="A113" s="16">
         <v>40.137500000000003</v>
       </c>
       <c r="B113" s="2">
@@ -3413,7 +3441,7 @@
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A114" s="17">
+      <c r="A114" s="16">
         <v>41.024999999999999</v>
       </c>
       <c r="B114" s="2">
@@ -3424,7 +3452,7 @@
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A115" s="17">
+      <c r="A115" s="16">
         <v>42.075000000000003</v>
       </c>
       <c r="B115" s="2">
@@ -3435,7 +3463,7 @@
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A116" s="17">
+      <c r="A116" s="16">
         <v>41.850000000000009</v>
       </c>
       <c r="B116" s="2">
@@ -3446,7 +3474,7 @@
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A117" s="17">
+      <c r="A117" s="16">
         <v>43.637499999999996</v>
       </c>
       <c r="B117" s="2">
@@ -3457,7 +3485,7 @@
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A118" s="17">
+      <c r="A118" s="16">
         <v>40.549999999999997</v>
       </c>
       <c r="B118" s="2">
@@ -3468,7 +3496,7 @@
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A119" s="17">
+      <c r="A119" s="16">
         <v>38.575000000000003</v>
       </c>
       <c r="B119" s="2">
@@ -3479,7 +3507,7 @@
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A120" s="17">
+      <c r="A120" s="16">
         <v>37.924999999999997</v>
       </c>
       <c r="B120" s="2">
@@ -3490,7 +3518,7 @@
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A121" s="17">
+      <c r="A121" s="16">
         <v>38.674999999999997</v>
       </c>
       <c r="B121" s="2">
@@ -3501,7 +3529,7 @@
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A122" s="17">
+      <c r="A122" s="16">
         <v>37.975000000000001</v>
       </c>
       <c r="B122" s="2">
@@ -3512,7 +3540,7 @@
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A123" s="17">
+      <c r="A123" s="16">
         <v>35.4</v>
       </c>
       <c r="B123" s="2">
@@ -3523,7 +3551,7 @@
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A124" s="17">
+      <c r="A124" s="16">
         <v>37.962499999999999</v>
       </c>
       <c r="B124" s="2">
@@ -3534,7 +3562,7 @@
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A125" s="17">
+      <c r="A125" s="16">
         <v>36.875</v>
       </c>
       <c r="B125" s="2">
@@ -3545,7 +3573,7 @@
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A126" s="17">
+      <c r="A126" s="16">
         <v>40.012500000000003</v>
       </c>
       <c r="B126" s="2">
@@ -3556,7 +3584,7 @@
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A127" s="17">
+      <c r="A127" s="16">
         <v>40.987500000000011</v>
       </c>
       <c r="B127" s="2">
@@ -3567,7 +3595,7 @@
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A128" s="17">
+      <c r="A128" s="16">
         <v>39.050000000000004</v>
       </c>
       <c r="B128" s="2">
@@ -3578,7 +3606,7 @@
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A129" s="17">
+      <c r="A129" s="16">
         <v>40.125</v>
       </c>
       <c r="B129" s="2">
@@ -3589,7 +3617,7 @@
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A130" s="17">
+      <c r="A130" s="16">
         <v>40.662500000000001</v>
       </c>
       <c r="B130" s="2">
@@ -3600,7 +3628,7 @@
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A131" s="17">
+      <c r="A131" s="16">
         <v>40.874999999999993</v>
       </c>
       <c r="B131" s="2">
@@ -3611,7 +3639,7 @@
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A132" s="17">
+      <c r="A132" s="16">
         <v>42.862499999999997</v>
       </c>
       <c r="B132" s="2">
@@ -3622,7 +3650,7 @@
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A133" s="17">
+      <c r="A133" s="16">
         <v>42.875</v>
       </c>
       <c r="B133" s="2">
@@ -3633,7 +3661,7 @@
       </c>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A134" s="17">
+      <c r="A134" s="16">
         <v>42.125</v>
       </c>
       <c r="B134" s="2">
@@ -3644,7 +3672,7 @@
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A135" s="17">
+      <c r="A135" s="16">
         <v>38.612499999999997</v>
       </c>
       <c r="B135" s="2">
@@ -3655,7 +3683,7 @@
       </c>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A136" s="17">
+      <c r="A136" s="16">
         <v>42.725000000000001</v>
       </c>
       <c r="B136" s="2">
@@ -3666,7 +3694,7 @@
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A137" s="17">
+      <c r="A137" s="16">
         <v>41.212499999999999</v>
       </c>
       <c r="B137" s="2">
@@ -3677,7 +3705,7 @@
       </c>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A138" s="17">
+      <c r="A138" s="16">
         <v>43.55</v>
       </c>
       <c r="B138" s="2">
@@ -3688,7 +3716,7 @@
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A139" s="17">
+      <c r="A139" s="16">
         <v>39.5625</v>
       </c>
       <c r="B139" s="2">
@@ -3699,7 +3727,7 @@
       </c>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A140" s="17">
+      <c r="A140" s="16">
         <v>41.349999999999994</v>
       </c>
       <c r="B140" s="2">
@@ -3710,7 +3738,7 @@
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A141" s="17">
+      <c r="A141" s="16">
         <v>37.574999999999996</v>
       </c>
       <c r="B141" s="2">
@@ -3721,7 +3749,7 @@
       </c>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A142" s="17">
+      <c r="A142" s="16">
         <v>42.737499999999997</v>
       </c>
       <c r="B142" s="2">
@@ -3732,7 +3760,7 @@
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A143" s="17">
+      <c r="A143" s="16">
         <v>42.262500000000003</v>
       </c>
       <c r="B143" s="2">
@@ -3743,7 +3771,7 @@
       </c>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A144" s="17">
+      <c r="A144" s="16">
         <v>40.987499999999997</v>
       </c>
       <c r="B144" s="2">
@@ -3754,7 +3782,7 @@
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A145" s="17">
+      <c r="A145" s="16">
         <v>42.462499999999999</v>
       </c>
       <c r="B145" s="2">
@@ -3765,7 +3793,7 @@
       </c>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A146" s="17">
+      <c r="A146" s="16">
         <v>38.650000000000006</v>
       </c>
       <c r="B146" s="2">
@@ -3776,7 +3804,7 @@
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A147" s="17">
+      <c r="A147" s="16">
         <v>41.524999999999999</v>
       </c>
       <c r="B147" s="2">
@@ -3787,7 +3815,7 @@
       </c>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A148" s="17">
+      <c r="A148" s="16">
         <v>42.462499999999999</v>
       </c>
       <c r="B148" s="2">
@@ -3798,7 +3826,7 @@
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A149" s="17">
+      <c r="A149" s="16">
         <v>43.074999999999989</v>
       </c>
       <c r="B149" s="2">
@@ -3809,7 +3837,7 @@
       </c>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A150" s="17">
+      <c r="A150" s="16">
         <v>42</v>
       </c>
       <c r="B150" s="2">
@@ -3820,7 +3848,7 @@
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A151" s="17">
+      <c r="A151" s="16">
         <v>42.862500000000011</v>
       </c>
       <c r="B151" s="2">
@@ -3831,7 +3859,7 @@
       </c>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A152" s="17">
+      <c r="A152" s="16">
         <v>43.137499999999996</v>
       </c>
       <c r="B152" s="2">
@@ -3842,7 +3870,7 @@
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A153" s="17">
+      <c r="A153" s="16">
         <v>43.25</v>
       </c>
       <c r="B153" s="2">
@@ -3853,7 +3881,7 @@
       </c>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A154" s="17">
+      <c r="A154" s="16">
         <v>41.737499999999997</v>
       </c>
       <c r="B154" s="2">
@@ -3864,7 +3892,7 @@
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A155" s="17">
+      <c r="A155" s="16">
         <v>42.35</v>
       </c>
       <c r="B155" s="2">
@@ -3875,7 +3903,7 @@
       </c>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A156" s="17">
+      <c r="A156" s="16">
         <v>41.625</v>
       </c>
       <c r="B156" s="2">
@@ -3886,7 +3914,7 @@
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A157" s="17">
+      <c r="A157" s="16">
         <v>40.525000000000006</v>
       </c>
       <c r="B157" s="2">
@@ -3897,7 +3925,7 @@
       </c>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A158" s="17">
+      <c r="A158" s="16">
         <v>42.737499999999997</v>
       </c>
       <c r="B158" s="2">
@@ -3908,7 +3936,7 @@
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A159" s="17">
+      <c r="A159" s="16">
         <v>40.237499999999997</v>
       </c>
       <c r="B159" s="2">
@@ -3919,7 +3947,7 @@
       </c>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A160" s="17">
+      <c r="A160" s="16">
         <v>41.150000000000006</v>
       </c>
       <c r="B160" s="2">
@@ -3930,7 +3958,7 @@
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A161" s="17">
+      <c r="A161" s="16">
         <v>43.612499999999997</v>
       </c>
       <c r="B161" s="2">
@@ -3941,7 +3969,7 @@
       </c>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A162" s="17">
+      <c r="A162" s="16">
         <v>44.512500000000003</v>
       </c>
       <c r="B162" s="2">
@@ -3952,7 +3980,7 @@
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A163" s="17">
+      <c r="A163" s="16">
         <v>40.525000000000006</v>
       </c>
       <c r="B163" s="2">
@@ -3963,7 +3991,7 @@
       </c>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A164" s="17">
+      <c r="A164" s="16">
         <v>40.25</v>
       </c>
       <c r="B164" s="2">
@@ -3974,7 +4002,7 @@
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A165" s="17">
+      <c r="A165" s="16">
         <v>40.475000000000001</v>
       </c>
       <c r="B165" s="2">
@@ -3985,7 +4013,7 @@
       </c>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A166" s="17">
+      <c r="A166" s="16">
         <v>42.6875</v>
       </c>
       <c r="B166" s="2">
@@ -3996,7 +4024,7 @@
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A167" s="17">
+      <c r="A167" s="16">
         <v>43.25</v>
       </c>
       <c r="B167" s="2">
@@ -4007,7 +4035,7 @@
       </c>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A168" s="17">
+      <c r="A168" s="16">
         <v>41.75</v>
       </c>
       <c r="B168" s="2">
@@ -4018,7 +4046,7 @@
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A169" s="17">
+      <c r="A169" s="16">
         <v>41.65</v>
       </c>
       <c r="B169" s="2">
@@ -4029,7 +4057,7 @@
       </c>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A170" s="17">
+      <c r="A170" s="16">
         <v>41.875</v>
       </c>
       <c r="B170" s="2">
@@ -4040,7 +4068,7 @@
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A171" s="17">
+      <c r="A171" s="16">
         <v>40.875</v>
       </c>
       <c r="B171" s="2">
@@ -4051,7 +4079,7 @@
       </c>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A172" s="17">
+      <c r="A172" s="16">
         <v>41.9375</v>
       </c>
       <c r="B172" s="2">
@@ -4062,7 +4090,7 @@
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A173" s="17">
+      <c r="A173" s="16">
         <v>40.537500000000001</v>
       </c>
       <c r="B173" s="2">
@@ -4073,7 +4101,7 @@
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A174" s="17">
+      <c r="A174" s="16">
         <v>42.8125</v>
       </c>
       <c r="B174" s="2">
@@ -4084,7 +4112,7 @@
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A175" s="17">
+      <c r="A175" s="16">
         <v>41.075000000000003</v>
       </c>
       <c r="B175" s="2">
@@ -4095,7 +4123,7 @@
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A176" s="17">
+      <c r="A176" s="16">
         <v>40.6875</v>
       </c>
       <c r="B176" s="2">
@@ -4106,7 +4134,7 @@
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A177" s="17">
+      <c r="A177" s="16">
         <v>40.783333333333339</v>
       </c>
       <c r="B177" s="2">
@@ -4117,7 +4145,7 @@
       </c>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A178" s="17">
+      <c r="A178" s="16">
         <v>40.975000000000001</v>
       </c>
       <c r="B178" s="2">
@@ -4128,7 +4156,7 @@
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A179" s="17">
+      <c r="A179" s="16">
         <v>41.8125</v>
       </c>
       <c r="B179" s="2">
@@ -4139,7 +4167,7 @@
       </c>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A180" s="17">
+      <c r="A180" s="16">
         <v>41.4375</v>
       </c>
       <c r="B180" s="2">
@@ -4150,7 +4178,7 @@
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A181" s="17">
+      <c r="A181" s="16">
         <v>41.1875</v>
       </c>
       <c r="B181" s="2">
@@ -4161,7 +4189,7 @@
       </c>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A182" s="17">
+      <c r="A182" s="16">
         <v>41.762499999999996</v>
       </c>
       <c r="B182" s="2">
@@ -4172,7 +4200,7 @@
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A183" s="17">
+      <c r="A183" s="16">
         <v>40.35</v>
       </c>
       <c r="B183" s="2">
@@ -4183,7 +4211,7 @@
       </c>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A184" s="17">
+      <c r="A184" s="16">
         <v>43.112500000000004</v>
       </c>
       <c r="B184" s="2">
@@ -4194,7 +4222,7 @@
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A185" s="17">
+      <c r="A185" s="16">
         <v>40.512500000000003</v>
       </c>
       <c r="B185" s="2">
@@ -4205,7 +4233,7 @@
       </c>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A186" s="17">
+      <c r="A186" s="16">
         <v>41.275000000000006</v>
       </c>
       <c r="B186" s="2">
@@ -4216,7 +4244,7 @@
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A187" s="17">
+      <c r="A187" s="16">
         <v>44.387499999999996</v>
       </c>
       <c r="B187" s="2">
@@ -4227,7 +4255,7 @@
       </c>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A188" s="17">
+      <c r="A188" s="16">
         <v>44.375</v>
       </c>
       <c r="B188" s="2">
@@ -4238,7 +4266,7 @@
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A189" s="17">
+      <c r="A189" s="16">
         <v>43.55</v>
       </c>
       <c r="B189" s="2">
@@ -4249,7 +4277,7 @@
       </c>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A190" s="17">
+      <c r="A190" s="16">
         <v>40.612500000000004</v>
       </c>
       <c r="B190" s="2">
@@ -4260,7 +4288,7 @@
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A191" s="17">
+      <c r="A191" s="16">
         <v>42.75</v>
       </c>
       <c r="B191" s="2">
@@ -4271,7 +4299,7 @@
       </c>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A192" s="17">
+      <c r="A192" s="16">
         <v>41.462500000000006</v>
       </c>
       <c r="B192" s="2">
@@ -4282,7 +4310,7 @@
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A193" s="17">
+      <c r="A193" s="16">
         <v>39.825000000000003</v>
       </c>
       <c r="B193" s="2">
@@ -4293,7 +4321,7 @@
       </c>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A194" s="17">
+      <c r="A194" s="16">
         <v>41.550000000000004</v>
       </c>
       <c r="B194" s="2">
@@ -4304,7 +4332,7 @@
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A195" s="17">
+      <c r="A195" s="16">
         <v>40.375</v>
       </c>
       <c r="B195" s="2">
@@ -4315,7 +4343,7 @@
       </c>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A196" s="17">
+      <c r="A196" s="16">
         <v>43.162500000000001</v>
       </c>
       <c r="B196" s="2">
@@ -4326,7 +4354,7 @@
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A197" s="17">
+      <c r="A197" s="16">
         <v>41.625</v>
       </c>
       <c r="B197" s="2">
@@ -4337,7 +4365,7 @@
       </c>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A198" s="17">
+      <c r="A198" s="16">
         <v>42.862499999999997</v>
       </c>
       <c r="B198" s="2">
@@ -4348,7 +4376,7 @@
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A199" s="17">
+      <c r="A199" s="16">
         <v>39.325000000000003</v>
       </c>
       <c r="B199" s="2">
@@ -4359,7 +4387,7 @@
       </c>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A200" s="17">
+      <c r="A200" s="16">
         <v>41.5625</v>
       </c>
       <c r="B200" s="2">
@@ -4370,7 +4398,7 @@
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A201" s="17">
+      <c r="A201" s="16">
         <v>42.2</v>
       </c>
       <c r="B201" s="2">
@@ -4381,7 +4409,7 @@
       </c>
     </row>
     <row r="202" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A202" s="17">
+      <c r="A202" s="16">
         <v>41.962500000000006</v>
       </c>
       <c r="B202" s="2">
@@ -4392,7 +4420,7 @@
       </c>
     </row>
     <row r="203" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A203" s="17">
+      <c r="A203" s="16">
         <v>40.45000000000001</v>
       </c>
       <c r="B203" s="2">
@@ -4408,7 +4436,7 @@
       </c>
     </row>
     <row r="206" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A206" s="17">
+      <c r="A206" s="16">
         <v>442.76</v>
       </c>
       <c r="B206" s="2">
@@ -4416,7 +4444,7 @@
       </c>
     </row>
     <row r="207" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A207" s="17">
+      <c r="A207" s="16">
         <v>415.65999999999997</v>
       </c>
       <c r="B207" s="2">
@@ -4424,7 +4452,7 @@
       </c>
     </row>
     <row r="208" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A208" s="17">
+      <c r="A208" s="16">
         <v>473.20000000000005</v>
       </c>
       <c r="B208" s="2">
@@ -4432,7 +4460,7 @@
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A209" s="17">
+      <c r="A209" s="16">
         <v>472.57999999999993</v>
       </c>
       <c r="B209" s="2">
@@ -4440,7 +4468,7 @@
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A210" s="17">
+      <c r="A210" s="16">
         <v>413.76</v>
       </c>
       <c r="B210" s="2">
@@ -4448,7 +4476,7 @@
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A211" s="17">
+      <c r="A211" s="16">
         <v>410.88</v>
       </c>
       <c r="B211" s="2">
@@ -4456,7 +4484,7 @@
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A212" s="17">
+      <c r="A212" s="16">
         <v>417.06000000000006</v>
       </c>
       <c r="B212" s="2">
@@ -4464,7 +4492,7 @@
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A213" s="17">
+      <c r="A213" s="16">
         <v>454.32000000000005</v>
       </c>
       <c r="B213" s="2">
@@ -4472,7 +4500,7 @@
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A214" s="17">
+      <c r="A214" s="16">
         <v>454.30000000000007</v>
       </c>
       <c r="B214" s="2">
@@ -4480,7 +4508,7 @@
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A215" s="17">
+      <c r="A215" s="16">
         <v>471.76</v>
       </c>
       <c r="B215" s="2">
@@ -4488,7 +4516,7 @@
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A216" s="17">
+      <c r="A216" s="16">
         <v>416.90000000000003</v>
       </c>
       <c r="B216" s="2">
@@ -4496,7 +4524,7 @@
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A217" s="17">
+      <c r="A217" s="16">
         <v>437.81999999999994</v>
       </c>
       <c r="B217" s="2">
@@ -4504,7 +4532,7 @@
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A218" s="17">
+      <c r="A218" s="16">
         <v>392.36</v>
       </c>
       <c r="B218" s="2">
@@ -4512,7 +4540,7 @@
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A219" s="17">
+      <c r="A219" s="16">
         <v>404.83999999999992</v>
       </c>
       <c r="B219" s="2">
@@ -4520,7 +4548,7 @@
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A220" s="17">
+      <c r="A220" s="16">
         <v>427.54000000000008</v>
       </c>
       <c r="B220" s="2">
@@ -4528,7 +4556,7 @@
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A221" s="17">
+      <c r="A221" s="16">
         <v>437.56000000000006</v>
       </c>
       <c r="B221" s="2">
@@ -4536,7 +4564,7 @@
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A222" s="17">
+      <c r="A222" s="16">
         <v>449.28</v>
       </c>
       <c r="B222" s="2">
@@ -4544,7 +4572,7 @@
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A223" s="17">
+      <c r="A223" s="16">
         <v>445.18</v>
       </c>
       <c r="B223" s="2">
@@ -4552,7 +4580,7 @@
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A224" s="17">
+      <c r="A224" s="16">
         <v>424.96000000000004</v>
       </c>
       <c r="B224" s="2">
@@ -4560,7 +4588,7 @@
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A225" s="17">
+      <c r="A225" s="16">
         <v>382.56</v>
       </c>
       <c r="B225" s="2">
@@ -4568,7 +4596,7 @@
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A226" s="17">
+      <c r="A226" s="16">
         <v>449.28</v>
       </c>
       <c r="B226" s="2">
@@ -4576,7 +4604,7 @@
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A227" s="17">
+      <c r="A227" s="16">
         <v>443.79999999999995</v>
       </c>
       <c r="B227" s="2">
@@ -4584,7 +4612,7 @@
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A228" s="17">
+      <c r="A228" s="16">
         <v>393.08</v>
       </c>
       <c r="B228" s="2">
@@ -4592,7 +4620,7 @@
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A229" s="17">
+      <c r="A229" s="16">
         <v>445.12</v>
       </c>
       <c r="B229" s="2">
@@ -4600,7 +4628,7 @@
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A230" s="17">
+      <c r="A230" s="16">
         <v>455.79999999999995</v>
       </c>
       <c r="B230" s="2">
@@ -4608,7 +4636,7 @@
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A231" s="17">
+      <c r="A231" s="16">
         <v>393.28</v>
       </c>
       <c r="B231" s="2">
@@ -4616,7 +4644,7 @@
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A232" s="17">
+      <c r="A232" s="16">
         <v>400.90000000000003</v>
       </c>
       <c r="B232" s="2">
@@ -4624,7 +4652,7 @@
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A233" s="17">
+      <c r="A233" s="16">
         <v>423.08</v>
       </c>
       <c r="B233" s="2">
@@ -4632,7 +4660,7 @@
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A234" s="17">
+      <c r="A234" s="16">
         <v>377.69999999999993</v>
       </c>
       <c r="B234" s="2">
@@ -4640,7 +4668,7 @@
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A235" s="17">
+      <c r="A235" s="16">
         <v>402.45999999999992</v>
       </c>
       <c r="B235" s="2">
@@ -4648,7 +4676,7 @@
       </c>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A236" s="17">
+      <c r="A236" s="16">
         <v>403.41999999999996</v>
       </c>
       <c r="B236" s="2">
@@ -4656,7 +4684,7 @@
       </c>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A237" s="17">
+      <c r="A237" s="16">
         <v>400.78000000000003</v>
       </c>
       <c r="B237" s="2">
@@ -4664,7 +4692,7 @@
       </c>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A238" s="17">
+      <c r="A238" s="16">
         <v>412.36</v>
       </c>
       <c r="B238" s="2">
@@ -4672,7 +4700,7 @@
       </c>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A239" s="17">
+      <c r="A239" s="16">
         <v>418.14</v>
       </c>
       <c r="B239" s="2">
@@ -4680,7 +4708,7 @@
       </c>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A240" s="17">
+      <c r="A240" s="16">
         <v>437.24</v>
       </c>
       <c r="B240" s="2">
@@ -4688,7 +4716,7 @@
       </c>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A241" s="17">
+      <c r="A241" s="16">
         <v>459.44000000000005</v>
       </c>
       <c r="B241" s="2">
@@ -4696,7 +4724,7 @@
       </c>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A242" s="17">
+      <c r="A242" s="16">
         <v>448.32000000000005</v>
       </c>
       <c r="B242" s="2">
@@ -4704,7 +4732,7 @@
       </c>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A243" s="17">
+      <c r="A243" s="16">
         <v>435.31999999999994</v>
       </c>
       <c r="B243" s="2">
@@ -4712,7 +4740,7 @@
       </c>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A244" s="17">
+      <c r="A244" s="16">
         <v>455.6</v>
       </c>
       <c r="B244" s="2">
@@ -4720,7 +4748,7 @@
       </c>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A245" s="17">
+      <c r="A245" s="16">
         <v>435.02</v>
       </c>
       <c r="B245" s="2">
@@ -4728,7 +4756,7 @@
       </c>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A246" s="17">
+      <c r="A246" s="16">
         <v>425.88</v>
       </c>
       <c r="B246" s="2">
@@ -4736,7 +4764,7 @@
       </c>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A247" s="17">
+      <c r="A247" s="16">
         <v>437.41999999999996</v>
       </c>
       <c r="B247" s="2">
@@ -4744,7 +4772,7 @@
       </c>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A248" s="17">
+      <c r="A248" s="16">
         <v>424.68000000000006</v>
       </c>
       <c r="B248" s="2">
@@ -4752,7 +4780,7 @@
       </c>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A249" s="17">
+      <c r="A249" s="16">
         <v>350.74</v>
       </c>
       <c r="B249" s="2">
@@ -4760,7 +4788,7 @@
       </c>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A250" s="17">
+      <c r="A250" s="16">
         <v>406.46000000000004</v>
       </c>
       <c r="B250" s="2">
@@ -4768,7 +4796,7 @@
       </c>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A251" s="17">
+      <c r="A251" s="16">
         <v>399.58000000000004</v>
       </c>
       <c r="B251" s="2">
@@ -4776,7 +4804,7 @@
       </c>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A252" s="17">
+      <c r="A252" s="16">
         <v>410.6</v>
       </c>
       <c r="B252" s="2">
@@ -4784,7 +4812,7 @@
       </c>
     </row>
     <row r="253" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A253" s="17">
+      <c r="A253" s="16">
         <v>448.42000000000007</v>
       </c>
       <c r="B253" s="2">
@@ -4792,7 +4820,7 @@
       </c>
     </row>
     <row r="254" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A254" s="17">
+      <c r="A254" s="16">
         <v>471.02000000000004</v>
       </c>
       <c r="B254" s="2">
@@ -4800,7 +4828,7 @@
       </c>
     </row>
     <row r="255" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A255" s="17">
+      <c r="A255" s="16">
         <v>418.68</v>
       </c>
       <c r="B255" s="2">
@@ -4808,7 +4836,7 @@
       </c>
     </row>
     <row r="256" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A256" s="17">
+      <c r="A256" s="16">
         <v>373.98</v>
       </c>
       <c r="B256" s="2">
@@ -4816,7 +4844,7 @@
       </c>
     </row>
     <row r="257" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A257" s="17">
+      <c r="A257" s="16">
         <v>390.70000000000005</v>
       </c>
       <c r="B257" s="2">
@@ -4824,7 +4852,7 @@
       </c>
     </row>
     <row r="258" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A258" s="17">
+      <c r="A258" s="16">
         <v>463.22</v>
       </c>
       <c r="B258" s="2">
@@ -4832,7 +4860,7 @@
       </c>
     </row>
     <row r="259" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A259" s="17">
+      <c r="A259" s="16">
         <v>498.99999999999989</v>
       </c>
       <c r="B259" s="2">
@@ -4840,7 +4868,7 @@
       </c>
     </row>
     <row r="260" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A260" s="17">
+      <c r="A260" s="16">
         <v>389.5</v>
       </c>
       <c r="B260" s="2">
@@ -4848,7 +4876,7 @@
       </c>
     </row>
     <row r="261" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A261" s="17">
+      <c r="A261" s="16">
         <v>369.12</v>
       </c>
       <c r="B261" s="2">
@@ -4856,7 +4884,7 @@
       </c>
     </row>
     <row r="262" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A262" s="17">
+      <c r="A262" s="16">
         <v>384.1</v>
       </c>
       <c r="B262" s="2">
@@ -4864,7 +4892,7 @@
       </c>
     </row>
     <row r="263" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A263" s="17">
+      <c r="A263" s="16">
         <v>398.64</v>
       </c>
       <c r="B263" s="2">
@@ -4872,7 +4900,7 @@
       </c>
     </row>
     <row r="264" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A264" s="17">
+      <c r="A264" s="16">
         <v>383.46000000000004</v>
       </c>
       <c r="B264" s="2">
@@ -4880,7 +4908,7 @@
       </c>
     </row>
     <row r="265" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A265" s="17">
+      <c r="A265" s="16">
         <v>421.28</v>
       </c>
       <c r="B265" s="2">
@@ -4888,7 +4916,7 @@
       </c>
     </row>
     <row r="266" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A266" s="17">
+      <c r="A266" s="16">
         <v>356.52</v>
       </c>
       <c r="B266" s="2">
@@ -4896,7 +4924,7 @@
       </c>
     </row>
     <row r="267" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A267" s="17">
+      <c r="A267" s="16">
         <v>380.78</v>
       </c>
       <c r="B267" s="2">
@@ -4904,7 +4932,7 @@
       </c>
     </row>
     <row r="268" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A268" s="17">
+      <c r="A268" s="16">
         <v>406.80000000000007</v>
       </c>
       <c r="B268" s="2">
@@ -4912,7 +4940,7 @@
       </c>
     </row>
     <row r="269" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A269" s="17">
+      <c r="A269" s="16">
         <v>373.84000000000003</v>
       </c>
       <c r="B269" s="2">
@@ -4920,7 +4948,7 @@
       </c>
     </row>
     <row r="270" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A270" s="17">
+      <c r="A270" s="16">
         <v>358.16</v>
       </c>
       <c r="B270" s="2">
@@ -4928,7 +4956,7 @@
       </c>
     </row>
     <row r="271" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A271" s="17">
+      <c r="A271" s="16">
         <v>351.3</v>
       </c>
       <c r="B271" s="2">
@@ -4936,7 +4964,7 @@
       </c>
     </row>
     <row r="272" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A272" s="17">
+      <c r="A272" s="16">
         <v>436.98</v>
       </c>
       <c r="B272" s="2">
@@ -4944,7 +4972,7 @@
       </c>
     </row>
     <row r="273" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A273" s="17">
+      <c r="A273" s="16">
         <v>410.72</v>
       </c>
       <c r="B273" s="2">
@@ -4952,7 +4980,7 @@
       </c>
     </row>
     <row r="274" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A274" s="17">
+      <c r="A274" s="16">
         <v>410.12</v>
       </c>
       <c r="B274" s="2">
@@ -4960,7 +4988,7 @@
       </c>
     </row>
     <row r="275" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A275" s="17">
+      <c r="A275" s="16">
         <v>444.09999999999997</v>
       </c>
       <c r="B275" s="2">
@@ -4968,7 +4996,7 @@
       </c>
     </row>
     <row r="276" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A276" s="17">
+      <c r="A276" s="16">
         <v>474.68000000000006</v>
       </c>
       <c r="B276" s="2">
@@ -4976,7 +5004,7 @@
       </c>
     </row>
     <row r="277" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A277" s="17">
+      <c r="A277" s="16">
         <v>452.15999999999997</v>
       </c>
       <c r="B277" s="2">
@@ -4984,7 +5012,7 @@
       </c>
     </row>
     <row r="278" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A278" s="17">
+      <c r="A278" s="16">
         <v>395.98</v>
       </c>
       <c r="B278" s="2">
@@ -4992,7 +5020,7 @@
       </c>
     </row>
     <row r="279" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A279" s="17">
+      <c r="A279" s="16">
         <v>386.13999999999987</v>
       </c>
       <c r="B279" s="2">
@@ -5000,7 +5028,7 @@
       </c>
     </row>
     <row r="280" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A280" s="17">
+      <c r="A280" s="16">
         <v>386.72</v>
       </c>
       <c r="B280" s="2">
@@ -5008,7 +5036,7 @@
       </c>
     </row>
     <row r="281" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A281" s="17">
+      <c r="A281" s="16">
         <v>374.94000000000005</v>
       </c>
       <c r="B281" s="2">
@@ -5016,7 +5044,7 @@
       </c>
     </row>
     <row r="282" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A282" s="17">
+      <c r="A282" s="16">
         <v>365.3</v>
       </c>
       <c r="B282" s="2">
@@ -5024,7 +5052,7 @@
       </c>
     </row>
     <row r="283" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A283" s="17">
+      <c r="A283" s="16">
         <v>385.59999999999997</v>
       </c>
       <c r="B283" s="2">
@@ -5032,7 +5060,7 @@
       </c>
     </row>
     <row r="284" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A284" s="17">
+      <c r="A284" s="16">
         <v>407.04</v>
       </c>
       <c r="B284" s="2">
@@ -5040,7 +5068,7 @@
       </c>
     </row>
     <row r="285" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A285" s="17">
+      <c r="A285" s="16">
         <v>396.70000000000005</v>
       </c>
       <c r="B285" s="2">
@@ -5048,7 +5076,7 @@
       </c>
     </row>
     <row r="286" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A286" s="17">
+      <c r="A286" s="16">
         <v>416.86</v>
       </c>
       <c r="B286" s="2">
@@ -5056,7 +5084,7 @@
       </c>
     </row>
     <row r="287" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A287" s="17">
+      <c r="A287" s="16">
         <v>417.16</v>
       </c>
       <c r="B287" s="2">
@@ -5064,7 +5092,7 @@
       </c>
     </row>
     <row r="288" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A288" s="17">
+      <c r="A288" s="16">
         <v>388.41999999999996</v>
       </c>
       <c r="B288" s="2">
@@ -5072,7 +5100,7 @@
       </c>
     </row>
     <row r="289" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A289" s="17">
+      <c r="A289" s="16">
         <v>411.22</v>
       </c>
       <c r="B289" s="2">
@@ -5080,7 +5108,7 @@
       </c>
     </row>
     <row r="290" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A290" s="17">
+      <c r="A290" s="16">
         <v>464.53999999999996</v>
       </c>
       <c r="B290" s="2">
@@ -5088,7 +5116,7 @@
       </c>
     </row>
     <row r="291" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A291" s="17">
+      <c r="A291" s="16">
         <v>387.59999999999997</v>
       </c>
       <c r="B291" s="2">
@@ -5096,7 +5124,7 @@
       </c>
     </row>
     <row r="292" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A292" s="17">
+      <c r="A292" s="16">
         <v>400.72</v>
       </c>
       <c r="B292" s="2">
@@ -5104,7 +5132,7 @@
       </c>
     </row>
     <row r="293" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A293" s="17">
+      <c r="A293" s="16">
         <v>446.29999999999995</v>
       </c>
       <c r="B293" s="2">
@@ -5112,7 +5140,7 @@
       </c>
     </row>
     <row r="294" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A294" s="17">
+      <c r="A294" s="16">
         <v>432.28</v>
       </c>
       <c r="B294" s="2">
@@ -5120,7 +5148,7 @@
       </c>
     </row>
     <row r="295" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A295" s="17">
+      <c r="A295" s="16">
         <v>443.74</v>
       </c>
       <c r="B295" s="2">
@@ -5128,7 +5156,7 @@
       </c>
     </row>
     <row r="296" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A296" s="17">
+      <c r="A296" s="16">
         <v>355.24</v>
       </c>
       <c r="B296" s="2">
@@ -5136,7 +5164,7 @@
       </c>
     </row>
     <row r="297" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A297" s="17">
+      <c r="A297" s="16">
         <v>366.93999999999994</v>
       </c>
       <c r="B297" s="2">
@@ -5144,7 +5172,7 @@
       </c>
     </row>
     <row r="298" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A298" s="17">
+      <c r="A298" s="16">
         <v>411.02</v>
       </c>
       <c r="B298" s="2">
@@ -5152,7 +5180,7 @@
       </c>
     </row>
     <row r="299" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A299" s="17">
+      <c r="A299" s="16">
         <v>373.34000000000003</v>
       </c>
       <c r="B299" s="2">
@@ -5160,7 +5188,7 @@
       </c>
     </row>
     <row r="300" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A300" s="17">
+      <c r="A300" s="16">
         <v>383.52</v>
       </c>
       <c r="B300" s="2">
@@ -5168,7 +5196,7 @@
       </c>
     </row>
     <row r="301" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A301" s="17">
+      <c r="A301" s="16">
         <v>345.12</v>
       </c>
       <c r="B301" s="2">
@@ -5176,7 +5204,7 @@
       </c>
     </row>
     <row r="302" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A302" s="17">
+      <c r="A302" s="16">
         <v>397.74</v>
       </c>
       <c r="B302" s="2">
@@ -5184,7 +5212,7 @@
       </c>
     </row>
     <row r="303" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A303" s="17">
+      <c r="A303" s="16">
         <v>412.57999999999993</v>
       </c>
       <c r="B303" s="2">
@@ -5192,7 +5220,7 @@
       </c>
     </row>
     <row r="304" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A304" s="17">
+      <c r="A304" s="16">
         <v>401.28</v>
       </c>
       <c r="B304" s="2">
@@ -5200,7 +5228,7 @@
       </c>
     </row>
     <row r="305" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A305" s="17">
+      <c r="A305" s="16">
         <v>415.72</v>
       </c>
       <c r="B305" s="2">
@@ -5208,7 +5236,7 @@
       </c>
     </row>
     <row r="306" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A306" s="17">
+      <c r="A306" s="16">
         <v>382.09999999999991</v>
       </c>
       <c r="B306" s="2">
@@ -5216,7 +5244,7 @@
       </c>
     </row>
     <row r="307" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A307" s="17">
+      <c r="A307" s="16">
         <v>434.02</v>
       </c>
       <c r="B307" s="2">
@@ -5224,7 +5252,7 @@
       </c>
     </row>
     <row r="308" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A308" s="17">
+      <c r="A308" s="16">
         <v>448.20000000000005</v>
       </c>
       <c r="B308" s="2">
@@ -5232,7 +5260,7 @@
       </c>
     </row>
     <row r="309" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A309" s="17">
+      <c r="A309" s="16">
         <v>374.78000000000003</v>
       </c>
       <c r="B309" s="2">
@@ -5240,7 +5268,7 @@
       </c>
     </row>
     <row r="310" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A310" s="17">
+      <c r="A310" s="16">
         <v>387.45999999999992</v>
       </c>
       <c r="B310" s="2">
@@ -5248,7 +5276,7 @@
       </c>
     </row>
     <row r="311" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A311" s="17">
+      <c r="A311" s="16">
         <v>429.70000000000005</v>
       </c>
       <c r="B311" s="2">
@@ -5256,7 +5284,7 @@
       </c>
     </row>
     <row r="312" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A312" s="17">
+      <c r="A312" s="16">
         <v>402.8</v>
       </c>
       <c r="B312" s="2">
@@ -5264,7 +5292,7 @@
       </c>
     </row>
     <row r="313" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A313" s="17">
+      <c r="A313" s="16">
         <v>439.34000000000003</v>
       </c>
       <c r="B313" s="2">
@@ -5272,7 +5300,7 @@
       </c>
     </row>
     <row r="314" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A314" s="17">
+      <c r="A314" s="16">
         <v>431.1</v>
       </c>
       <c r="B314" s="2">
@@ -5280,7 +5308,7 @@
       </c>
     </row>
     <row r="315" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A315" s="17">
+      <c r="A315" s="16">
         <v>429.58000000000004</v>
       </c>
       <c r="B315" s="2">
@@ -5288,7 +5316,7 @@
       </c>
     </row>
     <row r="316" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A316" s="17">
+      <c r="A316" s="16">
         <v>412.2</v>
       </c>
       <c r="B316" s="2">
@@ -5296,7 +5324,7 @@
       </c>
     </row>
     <row r="317" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A317" s="17">
+      <c r="A317" s="16">
         <v>429.94</v>
       </c>
       <c r="B317" s="2">
@@ -5304,7 +5332,7 @@
       </c>
     </row>
     <row r="318" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A318" s="17">
+      <c r="A318" s="16">
         <v>377.53999999999996</v>
       </c>
       <c r="B318" s="2">
@@ -5312,7 +5340,7 @@
       </c>
     </row>
     <row r="319" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A319" s="17">
+      <c r="A319" s="16">
         <v>429.36</v>
       </c>
       <c r="B319" s="2">
@@ -5320,7 +5348,7 @@
       </c>
     </row>
     <row r="320" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A320" s="17">
+      <c r="A320" s="16">
         <v>457.64000000000004</v>
       </c>
       <c r="B320" s="2">
@@ -5328,7 +5356,7 @@
       </c>
     </row>
     <row r="321" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A321" s="17">
+      <c r="A321" s="16">
         <v>443.56000000000006</v>
       </c>
       <c r="B321" s="2">
@@ -5336,7 +5364,7 @@
       </c>
     </row>
     <row r="322" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A322" s="17">
+      <c r="A322" s="16">
         <v>405.5200000000001</v>
       </c>
       <c r="B322" s="2">
@@ -5344,7 +5372,7 @@
       </c>
     </row>
     <row r="323" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A323" s="17">
+      <c r="A323" s="16">
         <v>408.36</v>
       </c>
       <c r="B323" s="2">
@@ -5352,7 +5380,7 @@
       </c>
     </row>
     <row r="324" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A324" s="17">
+      <c r="A324" s="16">
         <v>445.6400000000001</v>
       </c>
       <c r="B324" s="2">
@@ -5360,7 +5388,7 @@
       </c>
     </row>
     <row r="325" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A325" s="17">
+      <c r="A325" s="16">
         <v>398.41999999999996</v>
       </c>
       <c r="B325" s="2">
@@ -5368,7 +5396,7 @@
       </c>
     </row>
     <row r="326" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A326" s="17">
+      <c r="A326" s="16">
         <v>374.20000000000005</v>
       </c>
       <c r="B326" s="2">
@@ -5376,7 +5404,7 @@
       </c>
     </row>
     <row r="327" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A327" s="17">
+      <c r="A327" s="16">
         <v>391.76</v>
       </c>
       <c r="B327" s="2">
@@ -5384,7 +5412,7 @@
       </c>
     </row>
     <row r="328" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A328" s="17">
+      <c r="A328" s="16">
         <v>371.86</v>
       </c>
       <c r="B328" s="2">
@@ -5392,7 +5420,7 @@
       </c>
     </row>
     <row r="329" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A329" s="17">
+      <c r="A329" s="16">
         <v>353.58000000000004</v>
       </c>
       <c r="B329" s="2">
@@ -5400,7 +5428,7 @@
       </c>
     </row>
     <row r="330" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A330" s="17">
+      <c r="A330" s="16">
         <v>341.1</v>
       </c>
       <c r="B330" s="2">
@@ -5408,7 +5436,7 @@
       </c>
     </row>
     <row r="331" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A331" s="17">
+      <c r="A331" s="16">
         <v>358.24</v>
       </c>
       <c r="B331" s="2">
@@ -5416,7 +5444,7 @@
       </c>
     </row>
     <row r="332" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A332" s="17">
+      <c r="A332" s="16">
         <v>343.56</v>
       </c>
       <c r="B332" s="2">
@@ -5424,7 +5452,7 @@
       </c>
     </row>
     <row r="333" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A333" s="17">
+      <c r="A333" s="16">
         <v>349.72</v>
       </c>
       <c r="B333" s="2">
@@ -5432,7 +5460,7 @@
       </c>
     </row>
     <row r="334" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A334" s="17">
+      <c r="A334" s="16">
         <v>374.52000000000004</v>
       </c>
       <c r="B334" s="2">
@@ -5440,7 +5468,7 @@
       </c>
     </row>
     <row r="335" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A335" s="17">
+      <c r="A335" s="16">
         <v>357.8</v>
       </c>
       <c r="B335" s="2">
@@ -5448,7 +5476,7 @@
       </c>
     </row>
     <row r="336" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A336" s="17">
+      <c r="A336" s="16">
         <v>354.78</v>
       </c>
       <c r="B336" s="2">
@@ -5456,7 +5484,7 @@
       </c>
     </row>
     <row r="337" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A337" s="17">
+      <c r="A337" s="16">
         <v>380.9</v>
       </c>
       <c r="B337" s="2">
@@ -5464,7 +5492,7 @@
       </c>
     </row>
     <row r="338" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A338" s="17">
+      <c r="A338" s="16">
         <v>434.44000000000005</v>
       </c>
       <c r="B338" s="2">
@@ -5472,7 +5500,7 @@
       </c>
     </row>
     <row r="339" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A339" s="17">
+      <c r="A339" s="16">
         <v>381.22</v>
       </c>
       <c r="B339" s="2">
@@ -5480,7 +5508,7 @@
       </c>
     </row>
     <row r="340" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A340" s="17">
+      <c r="A340" s="16">
         <v>376.66</v>
       </c>
       <c r="B340" s="2">
@@ -5488,7 +5516,7 @@
       </c>
     </row>
     <row r="341" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A341" s="17">
+      <c r="A341" s="16">
         <v>429.94</v>
       </c>
       <c r="B341" s="2">
@@ -5496,7 +5524,7 @@
       </c>
     </row>
     <row r="342" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A342" s="17">
+      <c r="A342" s="16">
         <v>401.44</v>
       </c>
       <c r="B342" s="2">
@@ -5504,7 +5532,7 @@
       </c>
     </row>
     <row r="343" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A343" s="17">
+      <c r="A343" s="16">
         <v>448.7</v>
       </c>
       <c r="B343" s="2">
@@ -5512,7 +5540,7 @@
       </c>
     </row>
     <row r="344" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A344" s="17">
+      <c r="A344" s="16">
         <v>416.1</v>
       </c>
       <c r="B344" s="2">
@@ -5520,7 +5548,7 @@
       </c>
     </row>
     <row r="345" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A345" s="17">
+      <c r="A345" s="16">
         <v>362.32</v>
       </c>
       <c r="B345" s="2">
@@ -5528,7 +5556,7 @@
       </c>
     </row>
     <row r="346" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A346" s="17">
+      <c r="A346" s="16">
         <v>407.20000000000005</v>
       </c>
       <c r="B346" s="2">
@@ -5536,7 +5564,7 @@
       </c>
     </row>
     <row r="347" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A347" s="17">
+      <c r="A347" s="16">
         <v>386.66</v>
       </c>
       <c r="B347" s="2">
@@ -5544,7 +5572,7 @@
       </c>
     </row>
     <row r="348" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A348" s="17">
+      <c r="A348" s="16">
         <v>405.57999999999993</v>
       </c>
       <c r="B348" s="2">
@@ -5552,7 +5580,7 @@
       </c>
     </row>
     <row r="349" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A349" s="17">
+      <c r="A349" s="16">
         <v>397.46000000000004</v>
       </c>
       <c r="B349" s="2">

</xml_diff>